<commit_message>
Ajout des sous-totaux par enveloppe
</commit_message>
<xml_diff>
--- a/Feuille_depouillement absolu.xlsx
+++ b/Feuille_depouillement absolu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumnienacfr-my.sharepoint.com/personal/remi_barbero_alumni_enac_fr/Documents/Echange/Elections/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{66ED1F1D-0102-45AF-B77B-5DC36EB7394B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2D025CD-F926-4009-85E0-9F9430AFE173}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{66ED1F1D-0102-45AF-B77B-5DC36EB7394B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20B027A3-A203-428E-AEFC-1938A180F2DF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="39">
   <si>
     <t>Candidat 1</t>
   </si>
@@ -133,6 +133,24 @@
   <si>
     <t>_____</t>
   </si>
+  <si>
+    <t>Sous-total</t>
+  </si>
+  <si>
+    <t>Enveloppe 1</t>
+  </si>
+  <si>
+    <t>Enveloppe 2</t>
+  </si>
+  <si>
+    <t>Enveloppe 3</t>
+  </si>
+  <si>
+    <t>Enveloppe 4</t>
+  </si>
+  <si>
+    <t>Enveloppe 5</t>
+  </si>
 </sst>
 </file>
 
@@ -210,7 +228,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="54">
+  <borders count="64">
     <border>
       <left/>
       <right/>
@@ -923,11 +941,157 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1130,6 +1294,42 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1148,18 +1348,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1175,10 +1396,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1469,187 +1686,185 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:N70"/>
+  <dimension ref="B1:O77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" style="2" customWidth="1"/>
-    <col min="3" max="11" width="11.42578125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" style="1" customWidth="1"/>
-    <col min="13" max="14" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="6.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" style="2" customWidth="1"/>
+    <col min="4" max="12" width="11.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" style="1" customWidth="1"/>
+    <col min="14" max="15" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.7109375" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="3"/>
+    <row r="1" spans="3:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E1" s="3"/>
-      <c r="F1" s="76" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="3"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
-    </row>
-    <row r="2" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="78" t="s">
+      <c r="O1" s="3"/>
+    </row>
+    <row r="2" spans="3:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="78"/>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="80"/>
+      <c r="E2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="6" t="s">
+      <c r="F2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="78" t="s">
+    <row r="3" spans="3:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="80"/>
+      <c r="E3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="77" t="s">
+      <c r="G3" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="4"/>
-    </row>
-    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="78" t="s">
+      <c r="H3" s="83"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="83"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="3:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="78"/>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="80"/>
+      <c r="E4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="79">
+      <c r="G4" s="81">
         <v>46082</v>
       </c>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="79"/>
-      <c r="J4" s="79"/>
-      <c r="L4" s="6" t="s">
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81"/>
+      <c r="K4" s="81"/>
+      <c r="M4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="78" t="s">
+    <row r="5" spans="3:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="78"/>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="80"/>
+      <c r="E5" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="8"/>
+    <row r="6" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="8"/>
-      <c r="D6" s="7"/>
-    </row>
-    <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="43">
+      <c r="D6" s="8"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="43">
         <v>1</v>
       </c>
-      <c r="D7" s="44">
+      <c r="E7" s="44">
         <v>2</v>
       </c>
-      <c r="E7" s="44">
+      <c r="F7" s="44">
         <v>3</v>
       </c>
-      <c r="F7" s="44">
+      <c r="G7" s="44">
         <v>4</v>
       </c>
-      <c r="G7" s="44">
+      <c r="H7" s="44">
         <v>5</v>
       </c>
-      <c r="H7" s="44">
+      <c r="I7" s="44">
         <v>6</v>
       </c>
-      <c r="I7" s="44">
+      <c r="J7" s="44">
         <v>7</v>
       </c>
-      <c r="J7" s="44">
+      <c r="K7" s="44">
         <v>8</v>
       </c>
-      <c r="K7" s="44">
+      <c r="L7" s="44">
         <v>9</v>
       </c>
-      <c r="L7" s="45">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="68"/>
-      <c r="C8" s="48" t="s">
+      <c r="M7" s="45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="3:15" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="68"/>
+      <c r="D8" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="E8" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="39" t="s">
+      <c r="F8" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="39" t="s">
+      <c r="G8" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="39" t="s">
+      <c r="H8" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="39" t="s">
+      <c r="I8" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="39" t="s">
+      <c r="J8" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="39" t="s">
+      <c r="K8" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="39" t="s">
+      <c r="L8" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L8" s="40" t="s">
+      <c r="M8" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="M8" s="41" t="s">
+      <c r="N8" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="42" t="s">
+      <c r="O8" s="42" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="63">
+    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C9" s="63">
         <v>0</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="10" t="s">
@@ -1673,24 +1888,24 @@
       <c r="K9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L9" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="M9" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="N9" s="13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="64">
-        <v>10</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="15" t="s">
+      <c r="L9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="M9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="N9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="O9" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C10" s="64">
+        <v>10</v>
+      </c>
+      <c r="D10" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="15" t="s">
@@ -1714,24 +1929,24 @@
       <c r="K10" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L10" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M10" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N10" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="64">
+      <c r="L10" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M10" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N10" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O10" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C11" s="64">
         <v>20</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="15" t="s">
@@ -1755,24 +1970,24 @@
       <c r="K11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L11" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M11" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N11" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="64">
+      <c r="L11" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M11" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N11" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O11" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C12" s="64">
         <v>30</v>
       </c>
-      <c r="C12" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="15" t="s">
@@ -1796,24 +2011,24 @@
       <c r="K12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L12" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M12" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N12" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="64">
+      <c r="L12" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M12" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N12" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O12" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C13" s="64">
         <v>40</v>
       </c>
-      <c r="C13" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="15" t="s">
@@ -1837,24 +2052,24 @@
       <c r="K13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L13" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M13" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N13" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="64">
+      <c r="L13" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M13" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N13" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O13" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C14" s="64">
         <v>50</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="15" t="s">
@@ -1878,24 +2093,24 @@
       <c r="K14" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L14" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M14" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N14" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="64">
+      <c r="L14" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M14" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N14" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O14" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C15" s="64">
         <v>60</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="15" t="s">
@@ -1919,24 +2134,24 @@
       <c r="K15" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L15" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M15" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N15" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="64">
+      <c r="L15" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M15" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N15" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O15" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C16" s="64">
         <v>70</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="15" t="s">
@@ -1960,24 +2175,24 @@
       <c r="K16" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L16" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M16" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N16" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="65">
+      <c r="L16" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M16" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N16" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O16" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C17" s="65">
         <v>80</v>
       </c>
-      <c r="C17" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="19" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="20" t="s">
@@ -2001,24 +2216,24 @@
       <c r="K17" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="L17" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="M17" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="N17" s="23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="55">
+      <c r="L17" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="M17" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="N17" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="O17" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="55">
         <v>90</v>
       </c>
-      <c r="C18" s="56" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="57" t="s">
+      <c r="D18" s="56" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="57" t="s">
@@ -2042,24 +2257,24 @@
       <c r="K18" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="L18" s="58" t="s">
-        <v>10</v>
-      </c>
-      <c r="M18" s="59" t="s">
-        <v>10</v>
-      </c>
-      <c r="N18" s="60" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="66">
+      <c r="L18" s="57" t="s">
+        <v>10</v>
+      </c>
+      <c r="M18" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="N18" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="O18" s="60" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C19" s="66">
         <v>100</v>
       </c>
-      <c r="C19" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="24" t="s">
         <v>10</v>
       </c>
       <c r="E19" s="25" t="s">
@@ -2083,24 +2298,24 @@
       <c r="K19" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="L19" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="M19" s="61" t="s">
-        <v>10</v>
-      </c>
-      <c r="N19" s="62" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="64">
+      <c r="L19" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="M19" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="N19" s="61" t="s">
+        <v>10</v>
+      </c>
+      <c r="O19" s="62" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C20" s="64">
         <v>110</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="15" t="s">
@@ -2124,24 +2339,24 @@
       <c r="K20" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L20" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M20" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N20" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="66">
+      <c r="L20" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M20" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N20" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O20" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C21" s="66">
         <v>120</v>
       </c>
-      <c r="C21" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E21" s="15" t="s">
@@ -2165,24 +2380,24 @@
       <c r="K21" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L21" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M21" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N21" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="64">
+      <c r="L21" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M21" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N21" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O21" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C22" s="64">
         <v>130</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E22" s="15" t="s">
@@ -2206,24 +2421,24 @@
       <c r="K22" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L22" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M22" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N22" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B23" s="66">
+      <c r="L22" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M22" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N22" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O22" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C23" s="66">
         <v>140</v>
       </c>
-      <c r="C23" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E23" s="15" t="s">
@@ -2247,24 +2462,24 @@
       <c r="K23" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L23" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M23" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N23" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="64">
+      <c r="L23" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M23" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N23" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O23" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C24" s="64">
         <v>150</v>
       </c>
-      <c r="C24" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E24" s="15" t="s">
@@ -2288,24 +2503,24 @@
       <c r="K24" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L24" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M24" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N24" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="66">
+      <c r="L24" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M24" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N24" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O24" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C25" s="66">
         <v>160</v>
       </c>
-      <c r="C25" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E25" s="15" t="s">
@@ -2329,24 +2544,24 @@
       <c r="K25" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L25" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M25" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N25" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="64">
+      <c r="L25" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M25" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N25" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O25" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C26" s="64">
         <v>170</v>
       </c>
-      <c r="C26" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E26" s="15" t="s">
@@ -2370,24 +2585,24 @@
       <c r="K26" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L26" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M26" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N26" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="67">
+      <c r="L26" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M26" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N26" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O26" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C27" s="67">
         <v>180</v>
       </c>
-      <c r="C27" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="19" t="s">
         <v>10</v>
       </c>
       <c r="E27" s="20" t="s">
@@ -2411,24 +2626,24 @@
       <c r="K27" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="L27" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="M27" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="N27" s="23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="49">
+      <c r="L27" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="M27" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="N27" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="O27" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="49">
         <v>190</v>
       </c>
-      <c r="C28" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="51" t="s">
+      <c r="D28" s="50" t="s">
         <v>10</v>
       </c>
       <c r="E28" s="51" t="s">
@@ -2452,24 +2667,24 @@
       <c r="K28" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="L28" s="52" t="s">
-        <v>10</v>
-      </c>
-      <c r="M28" s="53" t="s">
-        <v>10</v>
-      </c>
-      <c r="N28" s="54" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="63">
+      <c r="L28" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="M28" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="N28" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="O28" s="54" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C29" s="63">
         <v>200</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E29" s="10" t="s">
@@ -2493,24 +2708,24 @@
       <c r="K29" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L29" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="M29" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="N29" s="13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="64">
+      <c r="L29" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="M29" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="N29" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="O29" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C30" s="64">
         <v>210</v>
       </c>
-      <c r="C30" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="15" t="s">
+      <c r="D30" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E30" s="15" t="s">
@@ -2534,24 +2749,24 @@
       <c r="K30" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L30" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M30" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N30" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="64">
+      <c r="L30" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M30" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N30" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O30" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C31" s="64">
         <v>220</v>
       </c>
-      <c r="C31" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" s="15" t="s">
+      <c r="D31" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E31" s="15" t="s">
@@ -2575,24 +2790,24 @@
       <c r="K31" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L31" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M31" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N31" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B32" s="64">
+      <c r="L31" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M31" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N31" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O31" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C32" s="64">
         <v>230</v>
       </c>
-      <c r="C32" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E32" s="15" t="s">
@@ -2616,24 +2831,24 @@
       <c r="K32" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L32" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M32" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N32" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B33" s="64">
+      <c r="L32" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M32" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N32" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O32" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C33" s="64">
         <v>240</v>
       </c>
-      <c r="C33" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E33" s="15" t="s">
@@ -2657,24 +2872,24 @@
       <c r="K33" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L33" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M33" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N33" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B34" s="64">
+      <c r="L33" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M33" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N33" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O33" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C34" s="64">
         <v>250</v>
       </c>
-      <c r="C34" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E34" s="15" t="s">
@@ -2698,24 +2913,24 @@
       <c r="K34" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L34" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M34" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N34" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B35" s="64">
+      <c r="L34" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M34" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N34" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O34" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C35" s="64">
         <v>260</v>
       </c>
-      <c r="C35" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E35" s="15" t="s">
@@ -2739,24 +2954,24 @@
       <c r="K35" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L35" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M35" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N35" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B36" s="64">
+      <c r="L35" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M35" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N35" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O35" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C36" s="64">
         <v>270</v>
       </c>
-      <c r="C36" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" s="15" t="s">
+      <c r="D36" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E36" s="15" t="s">
@@ -2780,24 +2995,24 @@
       <c r="K36" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L36" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M36" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N36" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B37" s="65">
+      <c r="L36" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M36" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N36" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O36" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C37" s="65">
         <v>280</v>
       </c>
-      <c r="C37" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" s="20" t="s">
+      <c r="D37" s="19" t="s">
         <v>10</v>
       </c>
       <c r="E37" s="20" t="s">
@@ -2821,24 +3036,24 @@
       <c r="K37" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="L37" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="M37" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="N37" s="23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="55">
+      <c r="L37" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="M37" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="N37" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="O37" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="55">
         <v>290</v>
       </c>
-      <c r="C38" s="56" t="s">
-        <v>10</v>
-      </c>
-      <c r="D38" s="57" t="s">
+      <c r="D38" s="56" t="s">
         <v>10</v>
       </c>
       <c r="E38" s="57" t="s">
@@ -2862,24 +3077,24 @@
       <c r="K38" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="L38" s="58" t="s">
-        <v>10</v>
-      </c>
-      <c r="M38" s="59" t="s">
-        <v>10</v>
-      </c>
-      <c r="N38" s="60" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B39" s="66">
+      <c r="L38" s="57" t="s">
+        <v>10</v>
+      </c>
+      <c r="M38" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="N38" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="O38" s="60" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C39" s="66">
         <v>300</v>
       </c>
-      <c r="C39" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" s="25" t="s">
+      <c r="D39" s="24" t="s">
         <v>10</v>
       </c>
       <c r="E39" s="25" t="s">
@@ -2903,24 +3118,24 @@
       <c r="K39" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="L39" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="M39" s="61" t="s">
-        <v>10</v>
-      </c>
-      <c r="N39" s="62" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B40" s="64">
+      <c r="L39" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="M39" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="N39" s="61" t="s">
+        <v>10</v>
+      </c>
+      <c r="O39" s="62" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C40" s="64">
         <v>310</v>
       </c>
-      <c r="C40" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" s="15" t="s">
+      <c r="D40" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E40" s="15" t="s">
@@ -2944,24 +3159,24 @@
       <c r="K40" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L40" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M40" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N40" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B41" s="64">
+      <c r="L40" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M40" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N40" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O40" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C41" s="64">
         <v>320</v>
       </c>
-      <c r="C41" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" s="15" t="s">
+      <c r="D41" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E41" s="15" t="s">
@@ -2985,24 +3200,24 @@
       <c r="K41" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L41" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M41" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N41" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B42" s="64">
+      <c r="L41" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M41" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N41" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O41" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C42" s="64">
         <v>330</v>
       </c>
-      <c r="C42" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D42" s="15" t="s">
+      <c r="D42" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E42" s="15" t="s">
@@ -3026,24 +3241,24 @@
       <c r="K42" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L42" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M42" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N42" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B43" s="64">
+      <c r="L42" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M42" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N42" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O42" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C43" s="64">
         <v>340</v>
       </c>
-      <c r="C43" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" s="15" t="s">
+      <c r="D43" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E43" s="15" t="s">
@@ -3067,24 +3282,24 @@
       <c r="K43" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L43" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M43" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N43" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B44" s="64">
+      <c r="L43" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M43" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N43" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O43" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C44" s="64">
         <v>350</v>
       </c>
-      <c r="C44" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D44" s="15" t="s">
+      <c r="D44" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E44" s="15" t="s">
@@ -3108,24 +3323,24 @@
       <c r="K44" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L44" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M44" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N44" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B45" s="64">
+      <c r="L44" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M44" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N44" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O44" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C45" s="64">
         <v>360</v>
       </c>
-      <c r="C45" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D45" s="15" t="s">
+      <c r="D45" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E45" s="15" t="s">
@@ -3149,24 +3364,24 @@
       <c r="K45" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L45" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M45" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N45" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B46" s="64">
+      <c r="L45" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M45" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N45" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O45" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C46" s="64">
         <v>370</v>
       </c>
-      <c r="C46" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D46" s="15" t="s">
+      <c r="D46" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E46" s="15" t="s">
@@ -3190,24 +3405,24 @@
       <c r="K46" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L46" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M46" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N46" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B47" s="65">
+      <c r="L46" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M46" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N46" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O46" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C47" s="65">
         <v>380</v>
       </c>
-      <c r="C47" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47" s="20" t="s">
+      <c r="D47" s="19" t="s">
         <v>10</v>
       </c>
       <c r="E47" s="20" t="s">
@@ -3231,24 +3446,24 @@
       <c r="K47" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="L47" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="M47" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="N47" s="23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="49">
+      <c r="L47" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="M47" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="N47" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="O47" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C48" s="49">
         <v>390</v>
       </c>
-      <c r="C48" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="D48" s="51" t="s">
+      <c r="D48" s="50" t="s">
         <v>10</v>
       </c>
       <c r="E48" s="51" t="s">
@@ -3272,24 +3487,24 @@
       <c r="K48" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="L48" s="52" t="s">
-        <v>10</v>
-      </c>
-      <c r="M48" s="53" t="s">
-        <v>10</v>
-      </c>
-      <c r="N48" s="54" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B49" s="63">
+      <c r="L48" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="M48" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="N48" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="O48" s="54" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C49" s="63">
         <v>400</v>
       </c>
-      <c r="C49" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D49" s="10" t="s">
+      <c r="D49" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E49" s="10" t="s">
@@ -3313,24 +3528,24 @@
       <c r="K49" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L49" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="M49" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="N49" s="13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B50" s="64">
+      <c r="L49" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="M49" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="N49" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="O49" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C50" s="64">
         <v>410</v>
       </c>
-      <c r="C50" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D50" s="15" t="s">
+      <c r="D50" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E50" s="15" t="s">
@@ -3354,24 +3569,24 @@
       <c r="K50" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L50" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M50" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N50" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B51" s="64">
+      <c r="L50" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M50" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N50" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O50" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C51" s="64">
         <v>420</v>
       </c>
-      <c r="C51" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D51" s="15" t="s">
+      <c r="D51" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E51" s="15" t="s">
@@ -3395,24 +3610,24 @@
       <c r="K51" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L51" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M51" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N51" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B52" s="64">
+      <c r="L51" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M51" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N51" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O51" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C52" s="64">
         <v>430</v>
       </c>
-      <c r="C52" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D52" s="15" t="s">
+      <c r="D52" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E52" s="15" t="s">
@@ -3436,24 +3651,24 @@
       <c r="K52" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L52" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M52" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N52" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B53" s="64">
+      <c r="L52" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M52" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N52" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O52" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C53" s="64">
         <v>440</v>
       </c>
-      <c r="C53" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D53" s="15" t="s">
+      <c r="D53" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E53" s="15" t="s">
@@ -3477,24 +3692,24 @@
       <c r="K53" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L53" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M53" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N53" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B54" s="64">
+      <c r="L53" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M53" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N53" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O53" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C54" s="64">
         <v>450</v>
       </c>
-      <c r="C54" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D54" s="15" t="s">
+      <c r="D54" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E54" s="15" t="s">
@@ -3518,24 +3733,24 @@
       <c r="K54" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L54" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M54" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N54" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B55" s="64">
+      <c r="L54" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M54" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N54" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O54" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C55" s="64">
         <v>460</v>
       </c>
-      <c r="C55" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D55" s="15" t="s">
+      <c r="D55" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E55" s="15" t="s">
@@ -3559,24 +3774,24 @@
       <c r="K55" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L55" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M55" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N55" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B56" s="64">
+      <c r="L55" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M55" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N55" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O55" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C56" s="64">
         <v>470</v>
       </c>
-      <c r="C56" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D56" s="15" t="s">
+      <c r="D56" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E56" s="15" t="s">
@@ -3600,24 +3815,24 @@
       <c r="K56" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L56" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M56" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N56" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B57" s="65">
+      <c r="L56" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M56" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N56" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O56" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C57" s="65">
         <v>480</v>
       </c>
-      <c r="C57" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D57" s="20" t="s">
+      <c r="D57" s="19" t="s">
         <v>10</v>
       </c>
       <c r="E57" s="20" t="s">
@@ -3641,24 +3856,24 @@
       <c r="K57" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="L57" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="M57" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="N57" s="23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="58" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="55">
+      <c r="L57" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="M57" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="N57" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="O57" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C58" s="55">
         <v>490</v>
       </c>
-      <c r="C58" s="56" t="s">
-        <v>10</v>
-      </c>
-      <c r="D58" s="57" t="s">
+      <c r="D58" s="56" t="s">
         <v>10</v>
       </c>
       <c r="E58" s="57" t="s">
@@ -3682,19 +3897,21 @@
       <c r="K58" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="L58" s="58" t="s">
-        <v>10</v>
-      </c>
-      <c r="M58" s="59" t="s">
-        <v>10</v>
-      </c>
-      <c r="N58" s="60" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="59" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="27"/>
-      <c r="C59" s="28"/>
+      <c r="L58" s="57" t="s">
+        <v>10</v>
+      </c>
+      <c r="M58" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="N58" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="O58" s="60" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C59" s="27"/>
       <c r="D59" s="28"/>
       <c r="E59" s="28"/>
       <c r="F59" s="28"/>
@@ -3704,215 +3921,341 @@
       <c r="J59" s="28"/>
       <c r="K59" s="28"/>
       <c r="L59" s="28"/>
-      <c r="M59" s="29"/>
-    </row>
-    <row r="60" spans="2:14" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C60" s="38" t="str">
-        <f t="shared" ref="C60:L60" si="0">C$8</f>
+      <c r="M59" s="28"/>
+      <c r="N59" s="29"/>
+    </row>
+    <row r="60" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="92" t="s">
+        <v>33</v>
+      </c>
+      <c r="C60" s="93"/>
+      <c r="D60" s="28"/>
+      <c r="E60" s="28"/>
+      <c r="F60" s="28"/>
+      <c r="G60" s="28"/>
+      <c r="H60" s="28"/>
+      <c r="I60" s="28"/>
+      <c r="J60" s="28"/>
+      <c r="K60" s="28"/>
+      <c r="L60" s="28"/>
+      <c r="M60" s="28"/>
+      <c r="N60" s="29"/>
+      <c r="O60" s="29"/>
+    </row>
+    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B61" s="94" t="s">
+        <v>34</v>
+      </c>
+      <c r="C61" s="95"/>
+      <c r="D61" s="76"/>
+      <c r="E61" s="71"/>
+      <c r="F61" s="71"/>
+      <c r="G61" s="71"/>
+      <c r="H61" s="71"/>
+      <c r="I61" s="71"/>
+      <c r="J61" s="71"/>
+      <c r="K61" s="71"/>
+      <c r="L61" s="71"/>
+      <c r="M61" s="98"/>
+      <c r="N61" s="100"/>
+      <c r="O61" s="72"/>
+    </row>
+    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B62" s="96" t="s">
+        <v>35</v>
+      </c>
+      <c r="C62" s="97"/>
+      <c r="D62" s="77"/>
+      <c r="E62" s="70"/>
+      <c r="F62" s="70"/>
+      <c r="G62" s="70"/>
+      <c r="H62" s="70"/>
+      <c r="I62" s="70"/>
+      <c r="J62" s="70"/>
+      <c r="K62" s="70"/>
+      <c r="L62" s="70"/>
+      <c r="M62" s="79"/>
+      <c r="N62" s="101"/>
+      <c r="O62" s="73"/>
+    </row>
+    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B63" s="96" t="s">
+        <v>36</v>
+      </c>
+      <c r="C63" s="97"/>
+      <c r="D63" s="77"/>
+      <c r="E63" s="70"/>
+      <c r="F63" s="70"/>
+      <c r="G63" s="70"/>
+      <c r="H63" s="70"/>
+      <c r="I63" s="70"/>
+      <c r="J63" s="70"/>
+      <c r="K63" s="70"/>
+      <c r="L63" s="70"/>
+      <c r="M63" s="79"/>
+      <c r="N63" s="101"/>
+      <c r="O63" s="73"/>
+    </row>
+    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B64" s="96" t="s">
+        <v>37</v>
+      </c>
+      <c r="C64" s="97"/>
+      <c r="D64" s="77"/>
+      <c r="E64" s="70"/>
+      <c r="F64" s="70"/>
+      <c r="G64" s="70"/>
+      <c r="H64" s="70"/>
+      <c r="I64" s="70"/>
+      <c r="J64" s="70"/>
+      <c r="K64" s="70"/>
+      <c r="L64" s="70"/>
+      <c r="M64" s="79"/>
+      <c r="N64" s="101"/>
+      <c r="O64" s="73"/>
+    </row>
+    <row r="65" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="90" t="s">
+        <v>38</v>
+      </c>
+      <c r="C65" s="91"/>
+      <c r="D65" s="78"/>
+      <c r="E65" s="74"/>
+      <c r="F65" s="74"/>
+      <c r="G65" s="74"/>
+      <c r="H65" s="74"/>
+      <c r="I65" s="74"/>
+      <c r="J65" s="74"/>
+      <c r="K65" s="74"/>
+      <c r="L65" s="74"/>
+      <c r="M65" s="99"/>
+      <c r="N65" s="102"/>
+      <c r="O65" s="75"/>
+    </row>
+    <row r="66" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C66" s="27"/>
+      <c r="D66" s="28"/>
+      <c r="E66" s="28"/>
+      <c r="F66" s="28"/>
+      <c r="G66" s="28"/>
+      <c r="H66" s="28"/>
+      <c r="I66" s="28"/>
+      <c r="J66" s="28"/>
+      <c r="K66" s="28"/>
+      <c r="L66" s="28"/>
+      <c r="M66" s="28"/>
+      <c r="N66" s="29"/>
+    </row>
+    <row r="67" spans="2:15" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D67" s="38" t="str">
+        <f t="shared" ref="D67:M67" si="0">D$8</f>
         <v>Candidat 1</v>
       </c>
-      <c r="D60" s="39" t="str">
+      <c r="E67" s="39" t="str">
         <f t="shared" si="0"/>
         <v>Candidat 2</v>
       </c>
-      <c r="E60" s="39" t="str">
+      <c r="F67" s="39" t="str">
         <f t="shared" si="0"/>
         <v>Candidat 3</v>
       </c>
-      <c r="F60" s="39" t="str">
+      <c r="G67" s="39" t="str">
         <f t="shared" si="0"/>
         <v>Candidat 4</v>
       </c>
-      <c r="G60" s="39" t="str">
+      <c r="H67" s="39" t="str">
         <f t="shared" si="0"/>
         <v>Candidat 5</v>
       </c>
-      <c r="H60" s="39" t="str">
+      <c r="I67" s="39" t="str">
         <f t="shared" si="0"/>
         <v>Candidat 6</v>
       </c>
-      <c r="I60" s="39" t="str">
+      <c r="J67" s="39" t="str">
         <f t="shared" si="0"/>
         <v>Candidat 7</v>
       </c>
-      <c r="J60" s="39" t="str">
+      <c r="K67" s="39" t="str">
         <f t="shared" si="0"/>
         <v>Candidat 8</v>
       </c>
-      <c r="K60" s="39" t="str">
+      <c r="L67" s="39" t="str">
         <f t="shared" si="0"/>
         <v>Candidat 9</v>
       </c>
-      <c r="L60" s="46" t="str">
+      <c r="M67" s="46" t="str">
         <f t="shared" si="0"/>
         <v>Candidat 10</v>
       </c>
-      <c r="M60" s="31"/>
-      <c r="N60" s="31"/>
-    </row>
-    <row r="61" spans="2:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="47" t="s">
+      <c r="N67" s="31"/>
+      <c r="O67" s="31"/>
+    </row>
+    <row r="68" spans="2:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C68" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="C61" s="35"/>
-      <c r="D61" s="36"/>
-      <c r="E61" s="36"/>
-      <c r="F61" s="36"/>
-      <c r="G61" s="36"/>
-      <c r="H61" s="36"/>
-      <c r="I61" s="36"/>
-      <c r="J61" s="36"/>
-      <c r="K61" s="36"/>
-      <c r="L61" s="37"/>
-    </row>
-    <row r="62" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="30"/>
-      <c r="C62" s="27"/>
-      <c r="D62" s="27"/>
-      <c r="E62" s="27"/>
-      <c r="F62" s="27"/>
-      <c r="G62" s="27"/>
-      <c r="H62" s="27"/>
-      <c r="I62" s="27"/>
-      <c r="J62" s="27"/>
-      <c r="K62" s="27"/>
-      <c r="L62" s="27"/>
-      <c r="M62" s="29"/>
-      <c r="N62" s="29"/>
-    </row>
-    <row r="63" spans="2:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="70" t="s">
+      <c r="D68" s="35"/>
+      <c r="E68" s="36"/>
+      <c r="F68" s="36"/>
+      <c r="G68" s="36"/>
+      <c r="H68" s="36"/>
+      <c r="I68" s="36"/>
+      <c r="J68" s="36"/>
+      <c r="K68" s="36"/>
+      <c r="L68" s="36"/>
+      <c r="M68" s="37"/>
+    </row>
+    <row r="69" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C69" s="30"/>
+      <c r="D69" s="27"/>
+      <c r="E69" s="27"/>
+      <c r="F69" s="27"/>
+      <c r="G69" s="27"/>
+      <c r="H69" s="27"/>
+      <c r="I69" s="27"/>
+      <c r="J69" s="27"/>
+      <c r="K69" s="27"/>
+      <c r="L69" s="27"/>
+      <c r="M69" s="27"/>
+      <c r="N69" s="29"/>
+      <c r="O69" s="29"/>
+    </row>
+    <row r="70" spans="2:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C70" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="C63" s="71"/>
-      <c r="D63" s="32"/>
-      <c r="E63" s="33" t="s">
+      <c r="D70" s="85"/>
+      <c r="E70" s="32"/>
+      <c r="F70" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="F63" s="69" t="s">
+      <c r="G70" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="G63" s="32"/>
-      <c r="H63" s="34" t="s">
+      <c r="H70" s="32"/>
+      <c r="I70" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="I63" s="47" t="s">
+      <c r="J70" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="J63" s="32"/>
-      <c r="K63" s="33" t="s">
+      <c r="K70" s="32"/>
+      <c r="L70" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="L63" s="47" t="s">
+      <c r="M70" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="M63" s="32">
-        <f>IF(ISNUMBER(D63-G63-J63),D63-G63-J63,"")</f>
-        <v>0</v>
-      </c>
-      <c r="N63" s="29"/>
-    </row>
-    <row r="65" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C65" s="72" t="s">
+      <c r="N70" s="32"/>
+      <c r="O70" s="29"/>
+    </row>
+    <row r="72" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D72" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="D65" s="72"/>
-      <c r="E65" s="72"/>
-      <c r="F65" s="72"/>
-      <c r="G65" s="72"/>
-      <c r="H65" s="72"/>
-      <c r="I65" s="72"/>
-      <c r="J65" s="72"/>
-      <c r="K65" s="72"/>
-      <c r="L65" s="72"/>
-      <c r="M65" s="72"/>
-      <c r="N65" s="72"/>
-    </row>
-    <row r="66" spans="3:14" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C66" s="73"/>
-      <c r="D66" s="74"/>
-      <c r="E66" s="75"/>
-      <c r="F66" s="73"/>
-      <c r="G66" s="74"/>
-      <c r="H66" s="75"/>
-      <c r="I66" s="73"/>
-      <c r="J66" s="74"/>
-      <c r="K66" s="75"/>
-      <c r="L66" s="73"/>
-      <c r="M66" s="74"/>
-      <c r="N66" s="75"/>
-    </row>
-    <row r="67" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C67" s="29"/>
-      <c r="D67" s="29"/>
-      <c r="E67" s="29"/>
-      <c r="F67" s="29"/>
-      <c r="G67" s="29"/>
-      <c r="H67" s="29"/>
-      <c r="I67" s="29"/>
-      <c r="J67" s="29"/>
-      <c r="K67" s="29"/>
-      <c r="L67" s="29"/>
-      <c r="M67" s="29"/>
-      <c r="N67" s="29"/>
-    </row>
-    <row r="68" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C68" s="29"/>
-      <c r="D68" s="29"/>
-      <c r="E68" s="29"/>
-      <c r="F68" s="29"/>
-      <c r="G68" s="29"/>
-      <c r="H68" s="29"/>
-      <c r="I68" s="29"/>
-      <c r="J68" s="29"/>
-      <c r="K68" s="29"/>
-      <c r="L68" s="29"/>
-      <c r="M68" s="29"/>
-      <c r="N68" s="29"/>
-    </row>
-    <row r="69" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C69" s="29"/>
-      <c r="D69" s="29"/>
-      <c r="E69" s="29"/>
-      <c r="F69" s="29"/>
-      <c r="G69" s="29"/>
-      <c r="H69" s="29"/>
-      <c r="I69" s="29"/>
-      <c r="J69" s="29"/>
-      <c r="K69" s="29"/>
-      <c r="L69" s="29"/>
-      <c r="M69" s="29"/>
-      <c r="N69" s="29"/>
-    </row>
-    <row r="70" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C70" s="29"/>
-      <c r="D70" s="29"/>
-      <c r="E70" s="29"/>
-      <c r="F70" s="29"/>
-      <c r="G70" s="29"/>
-      <c r="H70" s="29"/>
-      <c r="I70" s="29"/>
-      <c r="J70" s="29"/>
-      <c r="K70" s="29"/>
-      <c r="L70" s="29"/>
-      <c r="M70" s="29"/>
-      <c r="N70" s="29"/>
+      <c r="E72" s="86"/>
+      <c r="F72" s="86"/>
+      <c r="G72" s="86"/>
+      <c r="H72" s="86"/>
+      <c r="I72" s="86"/>
+      <c r="J72" s="86"/>
+      <c r="K72" s="86"/>
+      <c r="L72" s="86"/>
+      <c r="M72" s="86"/>
+      <c r="N72" s="86"/>
+      <c r="O72" s="86"/>
+    </row>
+    <row r="73" spans="2:15" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D73" s="87"/>
+      <c r="E73" s="88"/>
+      <c r="F73" s="89"/>
+      <c r="G73" s="87"/>
+      <c r="H73" s="88"/>
+      <c r="I73" s="89"/>
+      <c r="J73" s="87"/>
+      <c r="K73" s="88"/>
+      <c r="L73" s="89"/>
+      <c r="M73" s="87"/>
+      <c r="N73" s="88"/>
+      <c r="O73" s="89"/>
+    </row>
+    <row r="74" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D74" s="29"/>
+      <c r="E74" s="29"/>
+      <c r="F74" s="29"/>
+      <c r="G74" s="29"/>
+      <c r="H74" s="29"/>
+      <c r="I74" s="29"/>
+      <c r="J74" s="29"/>
+      <c r="K74" s="29"/>
+      <c r="L74" s="29"/>
+      <c r="M74" s="29"/>
+      <c r="N74" s="29"/>
+      <c r="O74" s="29"/>
+    </row>
+    <row r="75" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D75" s="29"/>
+      <c r="E75" s="29"/>
+      <c r="F75" s="29"/>
+      <c r="G75" s="29"/>
+      <c r="H75" s="29"/>
+      <c r="I75" s="29"/>
+      <c r="J75" s="29"/>
+      <c r="K75" s="29"/>
+      <c r="L75" s="29"/>
+      <c r="M75" s="29"/>
+      <c r="N75" s="29"/>
+      <c r="O75" s="29"/>
+    </row>
+    <row r="76" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D76" s="29"/>
+      <c r="E76" s="29"/>
+      <c r="F76" s="29"/>
+      <c r="G76" s="29"/>
+      <c r="H76" s="29"/>
+      <c r="I76" s="29"/>
+      <c r="J76" s="29"/>
+      <c r="K76" s="29"/>
+      <c r="L76" s="29"/>
+      <c r="M76" s="29"/>
+      <c r="N76" s="29"/>
+      <c r="O76" s="29"/>
+    </row>
+    <row r="77" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D77" s="29"/>
+      <c r="E77" s="29"/>
+      <c r="F77" s="29"/>
+      <c r="G77" s="29"/>
+      <c r="H77" s="29"/>
+      <c r="I77" s="29"/>
+      <c r="J77" s="29"/>
+      <c r="K77" s="29"/>
+      <c r="L77" s="29"/>
+      <c r="M77" s="29"/>
+      <c r="N77" s="29"/>
+      <c r="O77" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F3:J3"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
+  <mergeCells count="19">
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
     <mergeCell ref="B63:C63"/>
-    <mergeCell ref="C65:N65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="I66:K66"/>
-    <mergeCell ref="L66:N66"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="D72:O72"/>
+    <mergeCell ref="D73:F73"/>
+    <mergeCell ref="G73:I73"/>
+    <mergeCell ref="J73:L73"/>
+    <mergeCell ref="M73:O73"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>